<commit_message>
add cities into city list
</commit_message>
<xml_diff>
--- a/city-list.xlsx
+++ b/city-list.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100">
   <si>
     <t>city</t>
   </si>
@@ -197,6 +197,123 @@
   </si>
   <si>
     <t>https://www.tripadvisor.com/Hotels-g190454-Vienna-Hotels.html</t>
+  </si>
+  <si>
+    <t>Zurich</t>
+  </si>
+  <si>
+    <t>https://www.booking.com/searchresults.html?label=gen173nr-1DCAEoggJCAlhYSDNiBW5vcmVmaEiIAQGYATHCAQN4MTHIAQzYAQPoAQH4AQKSAgF5qAID;sid=5bbd1c1ae5a8c3b6a7dcce7d8431cdcc;class_interval=1&amp;dest_id=-2554935&amp;dest_type=city&amp;dtdisc=0&amp;group_adults=2&amp;group_children=0&amp;inac=0&amp;index_postcard=0&amp;label_click=undef&amp;no_rooms=1&amp;offset=0&amp;postcard=0&amp;raw_dest_type=city&amp;room1=A%2CA&amp;sb_price_type=total&amp;search_selected=1&amp;src=index&amp;src_elem=sb&amp;ss=Z%C3%BCrich%2C%20Canton%20of%20Zurich%2C%20Switzerland&amp;ss_all=0&amp;ss_raw=Zurich&amp;ssb=empty&amp;sshis=0&amp;</t>
+  </si>
+  <si>
+    <t>https://www.tripadvisor.com/Hotels-g188113-Zurich-Hotels.html</t>
+  </si>
+  <si>
+    <t>Budapest</t>
+  </si>
+  <si>
+    <t>https://www.booking.com/searchresults.html?label=gen173nr-1DCAEoggJCAlhYSDNiBW5vcmVmaEiIAQGYATHCAQN4MTHIAQzYAQPoAQH4AQKSAgF5qAID;sid=5bbd1c1ae5a8c3b6a7dcce7d8431cdcc;class_interval=1&amp;dest_id=-850553&amp;dest_type=city&amp;dtdisc=0&amp;group_adults=2&amp;group_children=0&amp;inac=0&amp;index_postcard=0&amp;label_click=undef&amp;no_rooms=1&amp;offset=0&amp;postcard=0&amp;raw_dest_type=city&amp;room1=A%2CA&amp;sb_price_type=total&amp;search_selected=1&amp;src=index&amp;src_elem=sb&amp;ss=Budapest%2C%20Pest%2C%20Hungary&amp;ss_all=0&amp;ss_raw=Budapest&amp;ssb=empty&amp;sshis=0&amp;</t>
+  </si>
+  <si>
+    <t>https://www.tripadvisor.com/Hotels-g274887-Budapest_Central_Hungary-Hotels.html</t>
+  </si>
+  <si>
+    <t>Warsaw</t>
+  </si>
+  <si>
+    <t>https://www.booking.com/searchresults.html?label=gen173nr-1DCAEoggJCAlhYSDNiBW5vcmVmaEiIAQGYATHCAQN4MTHIAQzYAQPoAQH4AQKSAgF5qAID;sid=5bbd1c1ae5a8c3b6a7dcce7d8431cdcc;class_interval=1;dest_id=-534433;dest_type=city;group_adults=2;group_children=0;label_click=undef;no_rooms=1;offset=0;qrhpp=a6c36cc6b36acf3bebd1204d1f69eaa8-city-0;room1=A%2CA;sb_price_type=total;search_pageview_id=f75442ee39c500ae;search_selected=0;src=index;src_elem=sb;ss=Warsaw;ss_raw=Warsaw;ssb=empty;srpos=1;origin=search</t>
+  </si>
+  <si>
+    <t>https://www.tripadvisor.com/Hotels-g274856-Warsaw_Mazovia_Province_Central_Poland-Hotels.html</t>
+  </si>
+  <si>
+    <t>Minsk</t>
+  </si>
+  <si>
+    <t>https://www.booking.com/searchresults.html?label=gen173nr-1DCAEoggJCAlhYSDNiBW5vcmVmaEiIAQGYATHCAQN4MTHIAQzYAQPoAQH4AQKSAgF5qAID;sid=5bbd1c1ae5a8c3b6a7dcce7d8431cdcc;class_interval=1&amp;dest_id=-1946324&amp;dest_type=city&amp;dtdisc=0&amp;group_adults=2&amp;group_children=0&amp;inac=0&amp;index_postcard=0&amp;label_click=undef&amp;no_rooms=1&amp;offset=0&amp;postcard=0&amp;raw_dest_type=city&amp;room1=A%2CA&amp;sb_price_type=total&amp;search_selected=1&amp;src=index&amp;src_elem=sb&amp;ss=Minsk%2C%20Minsk%20Region%2C%20Belarus&amp;ss_all=0&amp;ss_raw=Minsk&amp;ssb=empty&amp;sshis=0&amp;</t>
+  </si>
+  <si>
+    <t>https://www.tripadvisor.com/Hotels-g294448-Minsk-Hotels.html</t>
+  </si>
+  <si>
+    <t>Vilnius</t>
+  </si>
+  <si>
+    <t>https://www.booking.com/searchresults.html?label=gen173nr-1DCAEoggJCAlhYSDNiBW5vcmVmaEiIAQGYATHCAQN4MTHIAQzYAQPoAQH4AQKSAgF5qAID;sid=5bbd1c1ae5a8c3b6a7dcce7d8431cdcc;class_interval=1&amp;dest_id=3117&amp;dest_type=district&amp;dtdisc=0&amp;group_adults=2&amp;group_children=0&amp;inac=0&amp;index_postcard=0&amp;label_click=undef&amp;map=1&amp;no_rooms=1&amp;offset=0&amp;postcard=0&amp;raw_dest_type=district&amp;room1=A%2CA&amp;sb_price_type=total&amp;search_selected=1&amp;src=index&amp;src_elem=sb&amp;ss=Vilnius%20City%20Centre%2C%20Vilnius%2C%20Vilnius%20county%2C%20Lithuania&amp;ss_all=0&amp;ss_raw=Vilnius&amp;ssb=empty&amp;sshis=0&amp;#map_closed</t>
+  </si>
+  <si>
+    <t>https://www.tripadvisor.com/Hotels-g274951-Vilnius_Vilnius_County-Hotels.html</t>
+  </si>
+  <si>
+    <t>Riga</t>
+  </si>
+  <si>
+    <t>https://www.booking.com/searchresults.html?label=gen173nr-1DCAEoggJCAlhYSDNiBW5vcmVmaEiIAQGYATHCAQN4MTHIAQzYAQPoAQH4AQKSAgF5qAID;sid=5bbd1c1ae5a8c3b6a7dcce7d8431cdcc;class_interval=1&amp;dest_id=-3212216&amp;dest_type=city&amp;dtdisc=0&amp;group_adults=2&amp;group_children=0&amp;inac=0&amp;index_postcard=0&amp;label_click=undef&amp;no_rooms=1&amp;offset=0&amp;postcard=0&amp;raw_dest_type=city&amp;room1=A%2CA&amp;sb_price_type=total&amp;search_selected=1&amp;src=index&amp;src_elem=sb&amp;ss=R%C4%ABga%2C%20Vidzeme%2C%20Latvia&amp;ss_all=0&amp;ss_raw=Riga&amp;ssb=empty&amp;sshis=0&amp;</t>
+  </si>
+  <si>
+    <t>https://www.tripadvisor.com/Hotels-g274967-Riga_Riga_Region-Hotels.html</t>
+  </si>
+  <si>
+    <t>Tallinn</t>
+  </si>
+  <si>
+    <t>https://www.booking.com/searchresults.html?label=gen173nr-1DCAEoggJCAlhYSDNiBW5vcmVmaEiIAQGYATHCAQN4MTHIAQzYAQPoAQH4AQKSAgF5qAID;sid=5bbd1c1ae5a8c3b6a7dcce7d8431cdcc;class_interval=1&amp;dest_id=3816&amp;dest_type=district&amp;dtdisc=0&amp;group_adults=2&amp;group_children=0&amp;inac=0&amp;index_postcard=0&amp;label_click=undef&amp;map=1&amp;no_rooms=1&amp;offset=0&amp;postcard=0&amp;raw_dest_type=district&amp;room1=A%2CA&amp;sb_price_type=total&amp;search_selected=1&amp;src=index&amp;src_elem=sb&amp;ss=Tallinn%20City-Centre%2C%20Tallinn%2C%20Harjumaa%2C%20Estonia&amp;ss_all=0&amp;ss_raw=Tallinn&amp;ssb=empty&amp;sshis=0&amp;#map_opened</t>
+  </si>
+  <si>
+    <t>https://www.tripadvisor.com/Hotels-g274958-Tallinn_Harju_County-Hotels.html</t>
+  </si>
+  <si>
+    <t>Roma</t>
+  </si>
+  <si>
+    <t>https://www.booking.com/searchresults.html?label=gen173nr-1DCAEoggJCAlhYSDNiBW5vcmVmaEiIAQGYATHCAQN4MTHIAQzYAQPoAQH4AQKSAgF5qAID;sid=5bbd1c1ae5a8c3b6a7dcce7d8431cdcc;class_interval=1&amp;dest_id=-126693&amp;dest_type=city&amp;dtdisc=0&amp;group_adults=2&amp;group_children=0&amp;inac=0&amp;index_postcard=0&amp;label_click=undef&amp;no_rooms=1&amp;offset=0&amp;postcard=0&amp;raw_dest_type=city&amp;room1=A%2CA&amp;sb_price_type=total&amp;search_selected=1&amp;src=index&amp;src_elem=sb&amp;ss=Roma%2C%20Lazio%2C%20Italia&amp;ss_all=0&amp;ss_raw=ROma&amp;ssb=empty&amp;sshis=0&amp;</t>
+  </si>
+  <si>
+    <t>https://www.tripadvisor.com/Hotels-g187791-Rome_Lazio-Hotels.html</t>
+  </si>
+  <si>
+    <t>Kiev</t>
+  </si>
+  <si>
+    <t>https://www.booking.com/searchresults.html?label=gen173nr-1DCAEoggJCAlhYSDNiBW5vcmVmaEiIAQGYATHCAQN4MTHIAQzYAQPoAQH4AQKSAgF5qAID;sid=5bbd1c1ae5a8c3b6a7dcce7d8431cdcc;class_interval=1&amp;dest_id=-1044367&amp;dest_type=city&amp;dtdisc=0&amp;group_adults=2&amp;group_children=0&amp;inac=0&amp;index_postcard=0&amp;label_click=undef&amp;no_rooms=1&amp;offset=0&amp;postcard=0&amp;raw_dest_type=city&amp;room1=A%2CA&amp;sb_price_type=total&amp;search_selected=1&amp;src=index&amp;src_elem=sb&amp;ss=Kiev%2C%20Ukraine&amp;ss_all=0&amp;ss_raw=Kiev&amp;ssb=empty&amp;sshis=0&amp;</t>
+  </si>
+  <si>
+    <t>https://www.tripadvisor.com/Hotels-g294474-Kiev-Hotels.html</t>
+  </si>
+  <si>
+    <t>Bucharest</t>
+  </si>
+  <si>
+    <t>https://www.booking.com/searchresults.html?label=gen173nr-1DCAEoggJCAlhYSDNiBW5vcmVmaEiIAQGYATHCAQN4MTHIAQzYAQPoAQH4AQKSAgF5qAID;sid=5bbd1c1ae5a8c3b6a7dcce7d8431cdcc;class_interval=1&amp;dest_id=6817&amp;dest_type=district&amp;dtdisc=0&amp;group_adults=2&amp;group_children=0&amp;inac=0&amp;index_postcard=0&amp;label_click=undef&amp;map=1&amp;no_rooms=1&amp;offset=0&amp;postcard=0&amp;raw_dest_type=district&amp;room1=A%2CA&amp;sb_price_type=total&amp;search_selected=1&amp;src=index&amp;src_elem=sb&amp;ss=Bucharest%20City-Centre%2C%20Bucharest%2C%20Bucharest%20-%20Ilfov%20Region%2C%20Romania&amp;ss_all=0&amp;ss_raw=Bucharest&amp;ssb=empty&amp;sshis=0&amp;#map_closed</t>
+  </si>
+  <si>
+    <t>https://www.tripadvisor.com/Hotels-g294458-Bucharest-Hotels.html</t>
+  </si>
+  <si>
+    <t>Kharkiv</t>
+  </si>
+  <si>
+    <t>https://www.booking.com/searchresults.html?label=gen173nr-1DCAEoggJCAlhYSDNiBW5vcmVmaEiIAQGYATHCAQN4MTHIAQzYAQPoAQH4AQKSAgF5qAID;sid=5bbd1c1ae5a8c3b6a7dcce7d8431cdcc;class_interval=1&amp;dest_id=-1041320&amp;dest_type=city&amp;dtdisc=0&amp;group_adults=2&amp;group_children=0&amp;inac=0&amp;index_postcard=0&amp;label_click=undef&amp;no_rooms=1&amp;offset=0&amp;postcard=0&amp;raw_dest_type=city&amp;room1=A%2CA&amp;sb_price_type=total&amp;search_selected=1&amp;src=index&amp;src_elem=sb&amp;ss=Kharkov%2C%20Kharkiv%2C%20Ukraine&amp;ss_all=0&amp;ss_raw=Kharkiv&amp;ssb=empty&amp;sshis=0&amp;</t>
+  </si>
+  <si>
+    <t>https://www.tripadvisor.com/Hotels-g295369-Kharkiv_Kharkiv_Oblast-Hotels.html</t>
+  </si>
+  <si>
+    <t>Sofia</t>
+  </si>
+  <si>
+    <t>https://www.booking.com/searchresults.html?label=gen173nr-1DCAEoggJCAlhYSDNiBW5vcmVmaEiIAQGYATHCAQN4MTHIAQzYAQPoAQH4AQKSAgF5qAID;sid=5bbd1c1ae5a8c3b6a7dcce7d8431cdcc;class_interval=1&amp;dest_id=-838489&amp;dest_type=city&amp;dtdisc=0&amp;group_adults=2&amp;group_children=0&amp;inac=0&amp;index_postcard=0&amp;label_click=undef&amp;no_rooms=1&amp;offset=0&amp;postcard=0&amp;raw_dest_type=city&amp;room1=A%2CA&amp;sb_price_type=total&amp;search_selected=1&amp;src=index&amp;src_elem=sb&amp;ss=Sofia%2C%20Sofia%2C%20Bulgaria&amp;ss_all=0&amp;ss_raw=Sofia&amp;ssb=empty&amp;sshis=0&amp;</t>
+  </si>
+  <si>
+    <t>https://www.tripadvisor.com/Hotels-g294452-Sofia_Sofia_Region-Hotels.html</t>
+  </si>
+  <si>
+    <t>Cologne</t>
+  </si>
+  <si>
+    <t>https://www.booking.com/searchresults.html?label=gen173nr-1DCAEoggJCAlhYSDNiBW5vcmVmaEiIAQGYATHCAQN4MTHIAQzYAQPoAQH4AQKSAgF5qAID;sid=5bbd1c1ae5a8c3b6a7dcce7d8431cdcc;class_interval=1&amp;dest_id=-1810561&amp;dest_type=city&amp;dtdisc=0&amp;group_adults=2&amp;group_children=0&amp;inac=0&amp;index_postcard=0&amp;label_click=undef&amp;no_rooms=1&amp;offset=0&amp;postcard=0&amp;raw_dest_type=city&amp;room1=A%2CA&amp;sb_price_type=total&amp;search_selected=1&amp;src=index&amp;src_elem=sb&amp;ss=Cologne%2C%20North%20Rhine-Westphalia%2C%20Germany&amp;ss_all=0&amp;ss_raw=Cologne&amp;ssb=empty&amp;sshis=0&amp;</t>
+  </si>
+  <si>
+    <t>https://www.tripadvisor.com/Hotels-g187371-Cologne_North_Rhine_Westphalia-Hotels.html</t>
   </si>
 </sst>
 </file>
@@ -209,7 +326,7 @@
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -229,51 +346,6 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -302,8 +374,31 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -318,7 +413,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -332,8 +427,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -348,23 +452,28 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -379,12 +488,78 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -397,13 +572,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -415,151 +656,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -573,17 +682,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -607,7 +710,22 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -619,24 +737,6 @@
       </top>
       <bottom style="double">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -656,17 +756,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -675,145 +784,145 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -932,7 +1041,7 @@
             </a:prstGeom>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr wrap="square" anchor="ctr">
+            <a:bodyPr wrap="square" anchor="ctr" upright="1">
               <a:noAutofit/>
             </a:bodyPr>
             <a:p>
@@ -1002,7 +1111,7 @@
             </a:prstGeom>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr wrap="square" anchor="ctr">
+            <a:bodyPr wrap="square" anchor="ctr" upright="1">
               <a:noAutofit/>
             </a:bodyPr>
             <a:p>
@@ -1298,10 +1407,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="12.75" outlineLevelCol="5"/>
@@ -1313,7 +1422,6 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1"/>
       <c r="C1" t="s">
         <v>1</v>
       </c>
@@ -1541,6 +1649,149 @@
       </c>
       <c r="F25" s="2" t="s">
         <v>60</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" t="s">
+        <v>61</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" t="s">
+        <v>64</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" t="s">
+        <v>67</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" t="s">
+        <v>70</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" t="s">
+        <v>73</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" t="s">
+        <v>76</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" t="s">
+        <v>79</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" t="s">
+        <v>82</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" t="s">
+        <v>85</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" t="s">
+        <v>88</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" t="s">
+        <v>91</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" t="s">
+        <v>94</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" t="s">
+        <v>97</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -1579,6 +1830,32 @@
     <hyperlink ref="C24" r:id="rId36" display="https://www.booking.com/searchresults.html?label=gen173nr-1DCAEoggJCAlhYSDNiBW5vcmVmaEiIAQGYATHCAQN4MTHIAQzYAQPoAQH4AQKSAgF5qAID;sid=5bbd1c1ae5a8c3b6a7dcce7d8431cdcc;class_interval=1;dest_id=-553173;dest_type=city;group_adults=2;group_children=0;label_cli"/>
     <hyperlink ref="F25" r:id="rId37" display="https://www.tripadvisor.com/Hotels-g190454-Vienna-Hotels.html"/>
     <hyperlink ref="C25" r:id="rId38" display="https://www.booking.com/searchresults.html?label=gen173nr-1DCAEoggJCAlhYSDNiBW5vcmVmaEiIAQGYATHCAQN4MTHIAQzYAQPoAQH4AQKSAgF5qAID;sid=5bbd1c1ae5a8c3b6a7dcce7d8431cdcc;class_interval=1;dest_id=-1995499;dest_type=city;group_adults=2;group_children=0;label_cl"/>
+    <hyperlink ref="F26" r:id="rId39" display="https://www.tripadvisor.com/Hotels-g188113-Zurich-Hotels.html"/>
+    <hyperlink ref="C26" r:id="rId40" display="https://www.booking.com/searchresults.html?label=gen173nr-1DCAEoggJCAlhYSDNiBW5vcmVmaEiIAQGYATHCAQN4MTHIAQzYAQPoAQH4AQKSAgF5qAID;sid=5bbd1c1ae5a8c3b6a7dcce7d8431cdcc;class_interval=1&amp;dest_id=-2554935&amp;dest_type=city&amp;dtdisc=0&amp;group_adults=2&amp;group_children=0"/>
+    <hyperlink ref="F27" r:id="rId41" display="https://www.tripadvisor.com/Hotels-g274887-Budapest_Central_Hungary-Hotels.html"/>
+    <hyperlink ref="C27" r:id="rId42" display="https://www.booking.com/searchresults.html?label=gen173nr-1DCAEoggJCAlhYSDNiBW5vcmVmaEiIAQGYATHCAQN4MTHIAQzYAQPoAQH4AQKSAgF5qAID;sid=5bbd1c1ae5a8c3b6a7dcce7d8431cdcc;class_interval=1&amp;dest_id=-850553&amp;dest_type=city&amp;dtdisc=0&amp;group_adults=2&amp;group_children=0&amp;"/>
+    <hyperlink ref="F28" r:id="rId43" display="https://www.tripadvisor.com/Hotels-g274856-Warsaw_Mazovia_Province_Central_Poland-Hotels.html"/>
+    <hyperlink ref="C28" r:id="rId44" display="https://www.booking.com/searchresults.html?label=gen173nr-1DCAEoggJCAlhYSDNiBW5vcmVmaEiIAQGYATHCAQN4MTHIAQzYAQPoAQH4AQKSAgF5qAID;sid=5bbd1c1ae5a8c3b6a7dcce7d8431cdcc;class_interval=1;dest_id=-534433;dest_type=city;group_adults=2;group_children=0;label_cli"/>
+    <hyperlink ref="F29" r:id="rId45" display="https://www.tripadvisor.com/Hotels-g294448-Minsk-Hotels.html"/>
+    <hyperlink ref="C29" r:id="rId46" display="https://www.booking.com/searchresults.html?label=gen173nr-1DCAEoggJCAlhYSDNiBW5vcmVmaEiIAQGYATHCAQN4MTHIAQzYAQPoAQH4AQKSAgF5qAID;sid=5bbd1c1ae5a8c3b6a7dcce7d8431cdcc;class_interval=1&amp;dest_id=-1946324&amp;dest_type=city&amp;dtdisc=0&amp;group_adults=2&amp;group_children=0"/>
+    <hyperlink ref="F30" r:id="rId47" display="https://www.tripadvisor.com/Hotels-g274951-Vilnius_Vilnius_County-Hotels.html"/>
+    <hyperlink ref="C30" r:id="rId48" display="https://www.booking.com/searchresults.html?label=gen173nr-1DCAEoggJCAlhYSDNiBW5vcmVmaEiIAQGYATHCAQN4MTHIAQzYAQPoAQH4AQKSAgF5qAID;sid=5bbd1c1ae5a8c3b6a7dcce7d8431cdcc;class_interval=1&amp;dest_id=3117&amp;dest_type=district&amp;dtdisc=0&amp;group_adults=2&amp;group_children=0"/>
+    <hyperlink ref="F31" r:id="rId49" display="https://www.tripadvisor.com/Hotels-g274967-Riga_Riga_Region-Hotels.html"/>
+    <hyperlink ref="C31" r:id="rId50" display="https://www.booking.com/searchresults.html?label=gen173nr-1DCAEoggJCAlhYSDNiBW5vcmVmaEiIAQGYATHCAQN4MTHIAQzYAQPoAQH4AQKSAgF5qAID;sid=5bbd1c1ae5a8c3b6a7dcce7d8431cdcc;class_interval=1&amp;dest_id=-3212216&amp;dest_type=city&amp;dtdisc=0&amp;group_adults=2&amp;group_children=0"/>
+    <hyperlink ref="F32" r:id="rId51" display="https://www.tripadvisor.com/Hotels-g274958-Tallinn_Harju_County-Hotels.html"/>
+    <hyperlink ref="C32" r:id="rId52" display="https://www.booking.com/searchresults.html?label=gen173nr-1DCAEoggJCAlhYSDNiBW5vcmVmaEiIAQGYATHCAQN4MTHIAQzYAQPoAQH4AQKSAgF5qAID;sid=5bbd1c1ae5a8c3b6a7dcce7d8431cdcc;class_interval=1&amp;dest_id=3816&amp;dest_type=district&amp;dtdisc=0&amp;group_adults=2&amp;group_children=0"/>
+    <hyperlink ref="C33" r:id="rId53" display="https://www.booking.com/searchresults.html?label=gen173nr-1DCAEoggJCAlhYSDNiBW5vcmVmaEiIAQGYATHCAQN4MTHIAQzYAQPoAQH4AQKSAgF5qAID;sid=5bbd1c1ae5a8c3b6a7dcce7d8431cdcc;class_interval=1&amp;dest_id=-126693&amp;dest_type=city&amp;dtdisc=0&amp;group_adults=2&amp;group_children=0&amp;"/>
+    <hyperlink ref="F33" r:id="rId54" display="https://www.tripadvisor.com/Hotels-g187791-Rome_Lazio-Hotels.html"/>
+    <hyperlink ref="F34" r:id="rId55" display="https://www.tripadvisor.com/Hotels-g294474-Kiev-Hotels.html"/>
+    <hyperlink ref="C34" r:id="rId56" display="https://www.booking.com/searchresults.html?label=gen173nr-1DCAEoggJCAlhYSDNiBW5vcmVmaEiIAQGYATHCAQN4MTHIAQzYAQPoAQH4AQKSAgF5qAID;sid=5bbd1c1ae5a8c3b6a7dcce7d8431cdcc;class_interval=1&amp;dest_id=-1044367&amp;dest_type=city&amp;dtdisc=0&amp;group_adults=2&amp;group_children=0"/>
+    <hyperlink ref="F35" r:id="rId57" display="https://www.tripadvisor.com/Hotels-g294458-Bucharest-Hotels.html"/>
+    <hyperlink ref="C35" r:id="rId58" display="https://www.booking.com/searchresults.html?label=gen173nr-1DCAEoggJCAlhYSDNiBW5vcmVmaEiIAQGYATHCAQN4MTHIAQzYAQPoAQH4AQKSAgF5qAID;sid=5bbd1c1ae5a8c3b6a7dcce7d8431cdcc;class_interval=1&amp;dest_id=6817&amp;dest_type=district&amp;dtdisc=0&amp;group_adults=2&amp;group_children=0"/>
+    <hyperlink ref="F36" r:id="rId59" display="https://www.tripadvisor.com/Hotels-g295369-Kharkiv_Kharkiv_Oblast-Hotels.html"/>
+    <hyperlink ref="C36" r:id="rId60" display="https://www.booking.com/searchresults.html?label=gen173nr-1DCAEoggJCAlhYSDNiBW5vcmVmaEiIAQGYATHCAQN4MTHIAQzYAQPoAQH4AQKSAgF5qAID;sid=5bbd1c1ae5a8c3b6a7dcce7d8431cdcc;class_interval=1&amp;dest_id=-1041320&amp;dest_type=city&amp;dtdisc=0&amp;group_adults=2&amp;group_children=0"/>
+    <hyperlink ref="F37" r:id="rId61" display="https://www.tripadvisor.com/Hotels-g294452-Sofia_Sofia_Region-Hotels.html"/>
+    <hyperlink ref="C37" r:id="rId62" display="https://www.booking.com/searchresults.html?label=gen173nr-1DCAEoggJCAlhYSDNiBW5vcmVmaEiIAQGYATHCAQN4MTHIAQzYAQPoAQH4AQKSAgF5qAID;sid=5bbd1c1ae5a8c3b6a7dcce7d8431cdcc;class_interval=1&amp;dest_id=-838489&amp;dest_type=city&amp;dtdisc=0&amp;group_adults=2&amp;group_children=0&amp;"/>
+    <hyperlink ref="F38" r:id="rId63" display="https://www.tripadvisor.com/Hotels-g187371-Cologne_North_Rhine_Westphalia-Hotels.html"/>
+    <hyperlink ref="C38" r:id="rId64" display="https://www.booking.com/searchresults.html?label=gen173nr-1DCAEoggJCAlhYSDNiBW5vcmVmaEiIAQGYATHCAQN4MTHIAQzYAQPoAQH4AQKSAgF5qAID;sid=5bbd1c1ae5a8c3b6a7dcce7d8431cdcc;class_interval=1&amp;dest_id=-1810561&amp;dest_type=city&amp;dtdisc=0&amp;group_adults=2&amp;group_children=0"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>

</xml_diff>